<commit_message>
added class diagram and updated gantt
</commit_message>
<xml_diff>
--- a/Documents/Gantt Chart/Gantt_Weekly_Status2-2.xlsx
+++ b/Documents/Gantt Chart/Gantt_Weekly_Status2-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a98965/Dropbox/CS383/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Satan\Documents\GitHub\Trajectory\Documents\Gantt Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{680580A0-461F-9947-83EF-CBD5473E4C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4DD667-49FA-418F-B1F7-254509846866}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E656BF53-8C2F-9143-90A0-23AA440D0AB5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E656BF53-8C2F-9143-90A0-23AA440D0AB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -317,7 +315,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -345,7 +343,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,6 +395,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -611,19 +615,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -633,7 +638,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,23 +975,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1596FC7-FBA9-FA4D-A1A3-B3A3B96D1437}">
   <dimension ref="A1:BR76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="115" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:E86"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:68">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="58" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="58"/>
+      <c r="F1" s="55"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1005,7 +1011,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:68">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1197,13 +1203,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:68">
-      <c r="A3" s="59" t="s">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
       <c r="E3">
         <v>1</v>
       </c>
@@ -1218,13 +1224,13 @@
       </c>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:68">
-      <c r="A4" s="59" t="s">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A4" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4">
         <v>2</v>
       </c>
@@ -1253,13 +1259,13 @@
       <c r="X4" s="10"/>
       <c r="Y4" s="10"/>
     </row>
-    <row r="5" spans="1:68">
-      <c r="A5" s="59" t="s">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A5" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5">
         <v>3</v>
       </c>
@@ -1277,13 +1283,13 @@
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
     </row>
-    <row r="6" spans="1:68">
-      <c r="A6" s="57" t="s">
+    <row r="6" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A6" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
       <c r="E6">
         <v>4</v>
       </c>
@@ -1301,13 +1307,13 @@
       <c r="R6" s="15"/>
       <c r="S6" s="15"/>
     </row>
-    <row r="7" spans="1:68">
-      <c r="A7" s="57" t="s">
+    <row r="7" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A7" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
       <c r="E7">
         <v>5</v>
       </c>
@@ -1324,13 +1330,13 @@
       <c r="V7" s="15"/>
       <c r="W7" s="15"/>
     </row>
-    <row r="8" spans="1:68">
-      <c r="A8" s="57" t="s">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A8" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
       <c r="E8">
         <v>6</v>
       </c>
@@ -1345,13 +1351,13 @@
       </c>
       <c r="Y8" s="15"/>
     </row>
-    <row r="9" spans="1:68">
-      <c r="A9" s="57" t="s">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A9" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
       <c r="E9">
         <v>7</v>
       </c>
@@ -1367,13 +1373,13 @@
       </c>
       <c r="AA9" s="15"/>
     </row>
-    <row r="10" spans="1:68">
-      <c r="A10" s="57" t="s">
+    <row r="10" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A10" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
       <c r="E10">
         <v>8</v>
       </c>
@@ -1391,13 +1397,13 @@
       <c r="AE10" s="15"/>
       <c r="AF10" s="15"/>
     </row>
-    <row r="11" spans="1:68">
-      <c r="A11" s="57" t="s">
+    <row r="11" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A11" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
       <c r="E11">
         <v>9</v>
       </c>
@@ -1417,13 +1423,13 @@
       <c r="AH11" s="16"/>
       <c r="AI11" s="16"/>
     </row>
-    <row r="12" spans="1:68">
-      <c r="A12" s="55" t="s">
+    <row r="12" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A12" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12">
@@ -1433,13 +1439,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:68">
-      <c r="A13" s="57" t="s">
+    <row r="13" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A13" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
       <c r="F13">
         <f>SUM(F3:F11)</f>
         <v>28</v>
@@ -1448,7 +1454,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:68">
+    <row r="14" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1512,7 +1518,7 @@
       <c r="BG14" s="2"/>
       <c r="BH14" s="2"/>
     </row>
-    <row r="15" spans="1:68">
+    <row r="15" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
@@ -1536,7 +1542,7 @@
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
     </row>
-    <row r="16" spans="1:68">
+    <row r="16" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>15</v>
       </c>
@@ -1560,7 +1566,7 @@
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="1:70">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
@@ -1584,7 +1590,7 @@
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
     </row>
-    <row r="18" spans="1:70">
+    <row r="18" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
@@ -1612,7 +1618,7 @@
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
     </row>
-    <row r="19" spans="1:70">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>18</v>
       </c>
@@ -1642,7 +1648,7 @@
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
     </row>
-    <row r="20" spans="1:70">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>19</v>
       </c>
@@ -1664,13 +1670,13 @@
       <c r="P20" s="15"/>
       <c r="Q20" s="15"/>
     </row>
-    <row r="21" spans="1:70">
-      <c r="A21" s="56" t="s">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A21" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
       <c r="E21">
         <v>7</v>
       </c>
@@ -1689,7 +1695,7 @@
       <c r="V21" s="15"/>
       <c r="W21" s="15"/>
     </row>
-    <row r="22" spans="1:70">
+    <row r="22" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1714,7 +1720,7 @@
       <c r="AB22" s="15"/>
       <c r="AC22" s="15"/>
     </row>
-    <row r="23" spans="1:70">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
@@ -1739,7 +1745,7 @@
       <c r="AH23" s="15"/>
       <c r="AI23" s="15"/>
     </row>
-    <row r="24" spans="1:70">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
@@ -1770,7 +1776,7 @@
       <c r="AB24" s="15"/>
       <c r="AC24" s="15"/>
     </row>
-    <row r="25" spans="1:70">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
@@ -1793,7 +1799,7 @@
       <c r="M25" s="13"/>
       <c r="N25" s="13"/>
     </row>
-    <row r="26" spans="1:70">
+    <row r="26" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
@@ -1811,7 +1817,7 @@
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
     </row>
-    <row r="27" spans="1:70">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>43</v>
       </c>
@@ -1821,7 +1827,7 @@
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="1:70">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>25</v>
       </c>
@@ -1836,7 +1842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:70">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -1910,7 +1916,7 @@
       <c r="BQ29" s="2"/>
       <c r="BR29" s="2"/>
     </row>
-    <row r="30" spans="1:70">
+    <row r="30" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
@@ -1928,7 +1934,7 @@
       </c>
       <c r="I30" s="15"/>
     </row>
-    <row r="31" spans="1:70">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>28</v>
       </c>
@@ -1949,7 +1955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:70">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:65">
+    <row r="33" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>30</v>
       </c>
@@ -1992,7 +1998,7 @@
       </c>
       <c r="M33" s="15"/>
     </row>
-    <row r="34" spans="1:65">
+    <row r="34" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>31</v>
       </c>
@@ -2012,7 +2018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:65">
+    <row r="35" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>43</v>
       </c>
@@ -2022,7 +2028,7 @@
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
     </row>
-    <row r="36" spans="1:65">
+    <row r="36" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>25</v>
       </c>
@@ -2036,7 +2042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:65">
+    <row r="37" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
@@ -2105,13 +2111,13 @@
       <c r="BL37" s="2"/>
       <c r="BM37" s="2"/>
     </row>
-    <row r="38" spans="1:65">
-      <c r="A38" s="54" t="s">
+    <row r="38" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A38" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
       <c r="E38">
         <v>1</v>
       </c>
@@ -2167,13 +2173,13 @@
       <c r="AZ38" s="13"/>
       <c r="BA38" s="13"/>
     </row>
-    <row r="39" spans="1:65">
-      <c r="A39" s="53" t="s">
+    <row r="39" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A39" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="60"/>
       <c r="E39">
         <v>2</v>
       </c>
@@ -2231,13 +2237,13 @@
       <c r="AZ39" s="13"/>
       <c r="BA39" s="13"/>
     </row>
-    <row r="40" spans="1:65">
-      <c r="A40" s="53" t="s">
+    <row r="40" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A40" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="B40" s="53"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="53"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
       <c r="E40">
         <v>3</v>
       </c>
@@ -2295,13 +2301,13 @@
       <c r="AZ40" s="13"/>
       <c r="BA40" s="13"/>
     </row>
-    <row r="41" spans="1:65">
-      <c r="A41" s="53" t="s">
+    <row r="41" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A41" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
       <c r="E41">
         <v>4</v>
       </c>
@@ -2359,25 +2365,25 @@
       <c r="AZ41" s="13"/>
       <c r="BA41" s="13"/>
     </row>
-    <row r="42" spans="1:65">
-      <c r="A42" s="53" t="s">
+    <row r="42" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A42" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
       <c r="E42">
         <v>5</v>
       </c>
       <c r="F42" s="6">
         <v>3</v>
       </c>
-      <c r="H42" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
+      <c r="H42" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="I42" s="64"/>
+      <c r="J42" s="64"/>
+      <c r="K42" s="64"/>
       <c r="L42" s="13"/>
       <c r="M42" s="13"/>
       <c r="N42" s="13"/>
@@ -2421,13 +2427,13 @@
       <c r="AZ42" s="13"/>
       <c r="BA42" s="13"/>
     </row>
-    <row r="43" spans="1:65">
-      <c r="A43" s="53" t="s">
+    <row r="43" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A43" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
       <c r="E43">
         <v>6</v>
       </c>
@@ -2485,13 +2491,13 @@
       <c r="AZ43" s="13"/>
       <c r="BA43" s="13"/>
     </row>
-    <row r="44" spans="1:65">
-      <c r="A44" s="53" t="s">
+    <row r="44" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A44" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="60"/>
       <c r="E44">
         <v>7</v>
       </c>
@@ -2549,13 +2555,13 @@
       <c r="AZ44" s="13"/>
       <c r="BA44" s="13"/>
     </row>
-    <row r="45" spans="1:65">
-      <c r="A45" s="53" t="s">
+    <row r="45" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A45" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
       <c r="E45">
         <v>8</v>
       </c>
@@ -2611,13 +2617,13 @@
       <c r="AZ45" s="13"/>
       <c r="BA45" s="13"/>
     </row>
-    <row r="46" spans="1:65" s="24" customFormat="1">
-      <c r="A46" s="53" t="s">
+    <row r="46" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="53"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
       <c r="E46" s="24">
         <v>9</v>
       </c>
@@ -2673,13 +2679,13 @@
       <c r="AZ46" s="13"/>
       <c r="BA46" s="13"/>
     </row>
-    <row r="47" spans="1:65" s="24" customFormat="1">
-      <c r="A47" s="53" t="s">
+    <row r="47" spans="1:65" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="53"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
+      <c r="B47" s="60"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="60"/>
       <c r="E47" s="24">
         <v>10</v>
       </c>
@@ -2735,13 +2741,13 @@
       <c r="AZ47" s="13"/>
       <c r="BA47" s="13"/>
     </row>
-    <row r="48" spans="1:65">
-      <c r="A48" s="53" t="s">
+    <row r="48" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A48" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="53"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="60"/>
       <c r="E48">
         <v>11</v>
       </c>
@@ -2797,7 +2803,7 @@
       <c r="AZ48" s="13"/>
       <c r="BA48" s="13"/>
     </row>
-    <row r="49" spans="1:69">
+    <row r="49" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>43</v>
       </c>
@@ -2807,7 +2813,7 @@
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
     </row>
-    <row r="50" spans="1:69">
+    <row r="50" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>25</v>
       </c>
@@ -2822,7 +2828,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="51" spans="1:69">
+    <row r="51" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>34</v>
       </c>
@@ -2895,7 +2901,7 @@
       <c r="BP51" s="2"/>
       <c r="BQ51" s="2"/>
     </row>
-    <row r="52" spans="1:69">
+    <row r="52" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>35</v>
       </c>
@@ -2916,7 +2922,7 @@
       </c>
       <c r="I52" s="7"/>
     </row>
-    <row r="53" spans="1:69">
+    <row r="53" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>36</v>
       </c>
@@ -2940,7 +2946,7 @@
       </c>
       <c r="K53" s="7"/>
     </row>
-    <row r="54" spans="1:69">
+    <row r="54" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>37</v>
       </c>
@@ -2976,7 +2982,7 @@
       <c r="X54" s="7"/>
       <c r="Y54" s="7"/>
     </row>
-    <row r="55" spans="1:69">
+    <row r="55" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>38</v>
       </c>
@@ -3019,7 +3025,7 @@
       <c r="AS55" s="13"/>
       <c r="AT55" s="13"/>
     </row>
-    <row r="56" spans="1:69">
+    <row r="56" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>33</v>
       </c>
@@ -3035,7 +3041,7 @@
       <c r="G56">
         <v>2</v>
       </c>
-      <c r="H56" s="63" t="s">
+      <c r="H56" s="53" t="s">
         <v>41</v>
       </c>
       <c r="Z56" s="19">
@@ -3062,7 +3068,7 @@
       <c r="AS56" s="14"/>
       <c r="AT56" s="14"/>
     </row>
-    <row r="57" spans="1:69">
+    <row r="57" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>30</v>
       </c>
@@ -3088,7 +3094,7 @@
       <c r="AZ57" s="15"/>
       <c r="BA57" s="15"/>
     </row>
-    <row r="58" spans="1:69">
+    <row r="58" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>39</v>
       </c>
@@ -3114,7 +3120,7 @@
       <c r="BG58" s="15"/>
       <c r="BH58" s="15"/>
     </row>
-    <row r="59" spans="1:69">
+    <row r="59" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>40</v>
       </c>
@@ -3138,7 +3144,7 @@
       <c r="BL59" s="15"/>
       <c r="BM59" s="15"/>
     </row>
-    <row r="60" spans="1:69">
+    <row r="60" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
         <v>43</v>
       </c>
@@ -3155,7 +3161,7 @@
       </c>
       <c r="BO60" s="15"/>
     </row>
-    <row r="61" spans="1:69">
+    <row r="61" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>25</v>
       </c>
@@ -3166,7 +3172,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:69">
+    <row r="62" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>47</v>
       </c>
@@ -3238,10 +3244,10 @@
       <c r="BO62" s="2"/>
       <c r="BP62" s="2"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B66" s="23"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>54</v>
       </c>
@@ -3252,7 +3258,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C76" s="21">
         <v>22500</v>
       </c>
@@ -3262,12 +3268,17 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A7:D7"/>
@@ -3276,17 +3287,12 @@
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3301,9 +3307,9 @@
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="20"/>
       <c r="B1" s="20" t="s">
         <v>56</v>
@@ -3342,7 +3348,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="20" t="s">
         <v>59</v>
@@ -3358,7 +3364,7 @@
       </c>
       <c r="F2" s="20"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
       <c r="B3" s="20" t="s">
         <v>60</v>
@@ -3374,7 +3380,7 @@
       </c>
       <c r="F3" s="20"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>61</v>
       </c>
@@ -3394,7 +3400,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>62</v>
       </c>
@@ -3412,7 +3418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>63</v>
       </c>
@@ -3432,7 +3438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>64</v>
       </c>
@@ -3450,7 +3456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>65</v>
       </c>
@@ -3470,7 +3476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>47</v>
       </c>
@@ -3499,9 +3505,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="17" thickBot="1">
+    <row r="1" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -3524,40 +3530,40 @@
       <c r="T1" s="22"/>
       <c r="U1" s="22"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="25"/>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="63"/>
       <c r="J2" s="22"/>
-      <c r="K2" s="60" t="s">
+      <c r="K2" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="L2" s="61"/>
-      <c r="M2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="63"/>
       <c r="N2" s="22"/>
-      <c r="O2" s="60" t="s">
+      <c r="O2" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="63"/>
       <c r="R2" s="22"/>
-      <c r="S2" s="60" t="s">
+      <c r="S2" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="T2" s="61"/>
-      <c r="U2" s="62"/>
-    </row>
-    <row r="3" spans="1:21" ht="17" thickBot="1">
+      <c r="T2" s="62"/>
+      <c r="U2" s="63"/>
+    </row>
+    <row r="3" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="22"/>
       <c r="B3" s="22"/>
       <c r="C3" s="26" t="s">
@@ -3610,7 +3616,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="17" thickBot="1">
+    <row r="4" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="22"/>
       <c r="B4" s="32" t="s">
         <v>62</v>
@@ -3678,7 +3684,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="17" thickBot="1">
+    <row r="5" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22"/>
       <c r="B5" s="26" t="s">
         <v>61</v>
@@ -3746,7 +3752,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="17" thickBot="1">
+    <row r="6" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="22"/>
       <c r="B6" s="26" t="s">
         <v>64</v>
@@ -3814,7 +3820,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="17" thickBot="1">
+    <row r="7" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="22"/>
       <c r="B7" s="26" t="s">
         <v>63</v>
@@ -3882,7 +3888,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="17" thickBot="1">
+    <row r="8" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="22"/>
       <c r="B8" s="26" t="s">
         <v>65</v>
@@ -3950,7 +3956,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="17" thickBot="1">
+    <row r="9" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22"/>
       <c r="B9" s="26" t="s">
         <v>47</v>
@@ -4018,7 +4024,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="17" thickBot="1">
+    <row r="10" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
       <c r="B10" s="42" t="s">
         <v>25</v>
@@ -4088,7 +4094,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="22" t="s">
         <v>56</v>
@@ -4133,7 +4139,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="22" t="s">
         <v>59</v>
@@ -4148,7 +4154,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="22" t="s">
         <v>60</v>
@@ -4167,7 +4173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>61</v>
       </c>
@@ -4186,7 +4192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>62</v>
       </c>
@@ -4203,7 +4209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
         <v>63</v>
       </c>
@@ -4222,7 +4228,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
         <v>64</v>
       </c>
@@ -4239,7 +4245,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
         <v>65</v>
       </c>
@@ -4258,7 +4264,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="22" t="s">
         <v>47</v>
       </c>

</xml_diff>